<commit_message>
导出excel  BigDecimal 测试 success
</commit_message>
<xml_diff>
--- a/demo-easy-excel/src/main/resources/ExcelTest.xlsx
+++ b/demo-easy-excel/src/main/resources/ExcelTest.xlsx
@@ -109,17 +109,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>生日转换测试</t>
+          <t>生日</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>生日</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>年龄</t>
+          <t>存款</t>
         </is>
       </c>
     </row>
@@ -137,13 +132,8 @@
           <t>2011-11-11</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2011-11-11</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>9.0</v>
+      <c r="D2" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -160,13 +150,8 @@
           <t>2001-11-01</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2001-11-01</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>19.0</v>
+      <c r="D3" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="4">
@@ -183,13 +168,8 @@
           <t>2010-02-07</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2010-02-07</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>10.0</v>
+      <c r="D4" t="n">
+        <v>11.11</v>
       </c>
     </row>
     <row r="5">
@@ -206,13 +186,8 @@
           <t>2011-01-11</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2011-01-11</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>9.0</v>
+      <c r="D5" t="n">
+        <v>10.24</v>
       </c>
     </row>
     <row r="6">
@@ -229,13 +204,8 @@
           <t>2021-05-12</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2021-05-12</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>-1.0</v>
+      <c r="D6" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -252,12 +222,7 @@
           <t>2010-07-11</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2010-07-11</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
+      <c r="D7" t="n">
         <v>10.0</v>
       </c>
     </row>

</xml_diff>